<commit_message>
adapto el codigo a las nuevas series2
</commit_message>
<xml_diff>
--- a/Estacionalidad/outputs/datosPedidoMines.xlsx
+++ b/Estacionalidad/outputs/datosPedidoMines.xlsx
@@ -624,16 +624,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V2">
-        <v>0.00661321448579568</v>
+        <v>6613.21448579568</v>
       </c>
       <c r="W2">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X2">
-        <v>0.00562887581816071</v>
+        <v>5628.87581816071</v>
       </c>
       <c r="Y2">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z2">
         <v>0.1795534281295115</v>
@@ -707,16 +707,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V3">
-        <v>0.006742609783253349</v>
+        <v>6742.60978325335</v>
       </c>
       <c r="W3">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X3">
-        <v>0.00605655507557865</v>
+        <v>6056.55507557865</v>
       </c>
       <c r="Y3">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z3">
         <v>0.01956617280984818</v>
@@ -790,16 +790,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V4">
-        <v>0.00660814040585353</v>
+        <v>6608.14040585353</v>
       </c>
       <c r="W4">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X4">
-        <v>0.00592449290908389</v>
+        <v>5924.49290908389</v>
       </c>
       <c r="Y4">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z4">
         <v>-0.01994322402192128</v>
@@ -873,16 +873,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V5">
-        <v>0.00525029532111494</v>
+        <v>5250.29532111494</v>
       </c>
       <c r="W5">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X5">
-        <v>0.00615432364644905</v>
+        <v>6154.32364644905</v>
       </c>
       <c r="Y5">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z5">
         <v>-0.2054806649592075</v>
@@ -956,16 +956,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V6">
-        <v>0.00469808885642951</v>
+        <v>4698.08885642951</v>
       </c>
       <c r="W6">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X6">
-        <v>0.00489309134169378</v>
+        <v>4893.09134169378</v>
       </c>
       <c r="Y6">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z6">
         <v>-0.1051762674119757</v>
@@ -1039,16 +1039,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V7">
-        <v>0.00482285734277043</v>
+        <v>4822.85734277043</v>
       </c>
       <c r="W7">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X7">
-        <v>0.0048542152156692</v>
+        <v>4854.2152156692</v>
       </c>
       <c r="Y7">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z7">
         <v>0.02655728534596991</v>
@@ -1122,16 +1122,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V8">
-        <v>0.00521823857864479</v>
+        <v>5218.23857864479</v>
       </c>
       <c r="W8">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X8">
-        <v>0.0048204247653897</v>
+        <v>4820.4247653897</v>
       </c>
       <c r="Y8">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z8">
         <v>0.08198070309233718</v>
@@ -1205,16 +1205,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V9">
-        <v>0.00569603964760054</v>
+        <v>5696.03964760054</v>
       </c>
       <c r="W9">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X9">
-        <v>0.006209550960241919</v>
+        <v>6209.55096024192</v>
       </c>
       <c r="Y9">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z9">
         <v>0.09156366880408862</v>
@@ -1288,16 +1288,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V10">
-        <v>0.00538863016971005</v>
+        <v>5388.63016971005</v>
       </c>
       <c r="W10">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X10">
-        <v>0.004583746918722469</v>
+        <v>4583.74691872247</v>
       </c>
       <c r="Y10">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z10">
         <v>-0.05396898492797297</v>
@@ -1371,16 +1371,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V11">
-        <v>0.00535904466063268</v>
+        <v>5359.04466063268</v>
       </c>
       <c r="W11">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X11">
-        <v>0.00374877730159274</v>
+        <v>3748.77730159274</v>
       </c>
       <c r="Y11">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z11">
         <v>-0.005490358058653388</v>
@@ -1454,16 +1454,16 @@
         <v>204.6035390293532</v>
       </c>
       <c r="V12">
-        <v>0.00590682690192694</v>
+        <v>5906.82690192694</v>
       </c>
       <c r="W12">
-        <v>0.005663998741248403</v>
+        <v>5663.998741248403</v>
       </c>
       <c r="X12">
-        <v>0.00437958374358816</v>
+        <v>4379.58374358816</v>
       </c>
       <c r="Y12">
-        <v>0.005204876154197297</v>
+        <v>5204.876154197297</v>
       </c>
       <c r="Z12">
         <v>0.1022163978811832</v>
@@ -1519,16 +1519,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V13">
-        <v>0.00648727388066283</v>
+        <v>6487.27388066283</v>
       </c>
       <c r="W13">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X13">
-        <v>0.005781930748783779</v>
+        <v>5781.93074878378</v>
       </c>
       <c r="Y13">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z13">
         <v>0.3668963934433525</v>
@@ -1602,16 +1602,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V14">
-        <v>0.006921418860336</v>
+        <v>6921.418860336</v>
       </c>
       <c r="W14">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X14">
-        <v>0.00550968813040263</v>
+        <v>5509.68813040263</v>
       </c>
       <c r="Y14">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z14">
         <v>0.06692256064095936</v>
@@ -1685,16 +1685,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V15">
-        <v>0.00590942680679825</v>
+        <v>5909.42680679825</v>
       </c>
       <c r="W15">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X15">
-        <v>0.00616042048980422</v>
+        <v>6160.42048980422</v>
       </c>
       <c r="Y15">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z15">
         <v>-0.1462116473454725</v>
@@ -1768,16 +1768,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V16">
-        <v>0.005648124074111249</v>
+        <v>5648.12407411125</v>
       </c>
       <c r="W16">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X16">
-        <v>0.006524732013650111</v>
+        <v>6524.73201365011</v>
       </c>
       <c r="Y16">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z16">
         <v>-0.04421794891957975</v>
@@ -1851,16 +1851,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V17">
-        <v>0.00471729947807125</v>
+        <v>4717.29947807125</v>
       </c>
       <c r="W17">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X17">
-        <v>0.00496329064541387</v>
+        <v>4963.29064541387</v>
       </c>
       <c r="Y17">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z17">
         <v>-0.1648024341934217</v>
@@ -1934,16 +1934,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V18">
-        <v>0.00485992351553674</v>
+        <v>4859.92351553674</v>
       </c>
       <c r="W18">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X18">
-        <v>0.00503344295821556</v>
+        <v>5033.44295821556</v>
       </c>
       <c r="Y18">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z18">
         <v>0.03023425545240221</v>
@@ -2017,16 +2017,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V19">
-        <v>0.00476039348296788</v>
+        <v>4760.39348296788</v>
       </c>
       <c r="W19">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X19">
-        <v>0.00493490198066237</v>
+        <v>4934.90198066237</v>
       </c>
       <c r="Y19">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z19">
         <v>-0.02047975287073367</v>
@@ -2100,16 +2100,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V20">
-        <v>0.00524484519139536</v>
+        <v>5244.84519139536</v>
       </c>
       <c r="W20">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X20">
-        <v>0.0060397845467629</v>
+        <v>6039.7845467629</v>
       </c>
       <c r="Y20">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z20">
         <v>0.1017671564673783</v>
@@ -2183,16 +2183,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V21">
-        <v>0.00544725186238711</v>
+        <v>5447.25186238711</v>
       </c>
       <c r="W21">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X21">
-        <v>0.00465811142941392</v>
+        <v>4658.11142941392</v>
       </c>
       <c r="Y21">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z21">
         <v>0.03859154343083682</v>
@@ -2266,16 +2266,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V22">
-        <v>0.00524006655972614</v>
+        <v>5240.06655972614</v>
       </c>
       <c r="W22">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X22">
-        <v>0.00371021731730833</v>
+        <v>3710.21731730833</v>
       </c>
       <c r="Y22">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z22">
         <v>-0.03803483075412206</v>
@@ -2349,16 +2349,16 @@
         <v>188.9398326631116</v>
       </c>
       <c r="V23">
-        <v>0.00592065086828837</v>
+        <v>5920.65086828837</v>
       </c>
       <c r="W23">
-        <v>0.005559697689116471</v>
+        <v>5559.69768911647</v>
       </c>
       <c r="X23">
-        <v>0.00451040350092664</v>
+        <v>4510.40350092664</v>
       </c>
       <c r="Y23">
-        <v>0.005256993069213121</v>
+        <v>5256.993069213121</v>
       </c>
       <c r="Z23">
         <v>0.1298808518565455</v>
@@ -2414,16 +2414,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V24">
-        <v>0.006721603690400021</v>
+        <v>6721.60369040002</v>
       </c>
       <c r="W24">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X24">
-        <v>0.005858022603360769</v>
+        <v>5858.02260336077</v>
       </c>
       <c r="Y24">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z24">
         <v>0.3025303776414539</v>
@@ -2497,16 +2497,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V25">
-        <v>0.00686472896621875</v>
+        <v>6864.72896621875</v>
       </c>
       <c r="W25">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X25">
-        <v>0.005414030956652611</v>
+        <v>5414.03095665261</v>
       </c>
       <c r="Y25">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z25">
         <v>0.02129332260739281</v>
@@ -2580,16 +2580,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V26">
-        <v>0.00662281643790832</v>
+        <v>6622.81643790832</v>
       </c>
       <c r="W26">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X26">
-        <v>0.00634488177109433</v>
+        <v>6344.88177109433</v>
       </c>
       <c r="Y26">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z26">
         <v>-0.03523992418358812</v>
@@ -2663,16 +2663,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V27">
-        <v>0.0054857912013823</v>
+        <v>5485.7912013823</v>
       </c>
       <c r="W27">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X27">
-        <v>0.00562890878486934</v>
+        <v>5628.90878486934</v>
       </c>
       <c r="Y27">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z27">
         <v>-0.1716830365428528</v>
@@ -2746,16 +2746,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V28">
-        <v>0.00478708734213477</v>
+        <v>4787.08734213477</v>
       </c>
       <c r="W28">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X28">
-        <v>0.005129134553410791</v>
+        <v>5129.13455341079</v>
       </c>
       <c r="Y28">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z28">
         <v>-0.1273661051976371</v>
@@ -2829,16 +2829,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V29">
-        <v>0.00454100887052456</v>
+        <v>4541.00887052456</v>
       </c>
       <c r="W29">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X29">
-        <v>0.00459888995108813</v>
+        <v>4598.88995108813</v>
       </c>
       <c r="Y29">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z29">
         <v>-0.05140463376222271</v>
@@ -2912,16 +2912,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V30">
-        <v>0.00485662968648406</v>
+        <v>4856.62968648406</v>
       </c>
       <c r="W30">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X30">
-        <v>0.005277496336979879</v>
+        <v>5277.49633697988</v>
       </c>
       <c r="Y30">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z30">
         <v>0.06950455833904612</v>
@@ -2995,16 +2995,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V31">
-        <v>0.00553221265584878</v>
+        <v>5532.21265584878</v>
       </c>
       <c r="W31">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X31">
-        <v>0.00611153090635238</v>
+        <v>6111.53090635238</v>
       </c>
       <c r="Y31">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z31">
         <v>0.1391053082026943</v>
@@ -3078,16 +3078,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V32">
-        <v>0.00552128962398993</v>
+        <v>5521.28962398993</v>
       </c>
       <c r="W32">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X32">
-        <v>0.00410966252939906</v>
+        <v>4109.66252939906</v>
       </c>
       <c r="Y32">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z32">
         <v>-0.001974441789995507</v>
@@ -3161,16 +3161,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V33">
-        <v>0.004626605320893921</v>
+        <v>4626.60532089392</v>
       </c>
       <c r="W33">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X33">
-        <v>0.00309289026714018</v>
+        <v>3092.89026714018</v>
       </c>
       <c r="Y33">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z33">
         <v>-0.1620426320707066</v>
@@ -3244,16 +3244,16 @@
         <v>212.5384464893532</v>
       </c>
       <c r="V34">
-        <v>0.00598774499683763</v>
+        <v>5987.74499683763</v>
       </c>
       <c r="W34">
-        <v>0.005595228981147549</v>
+        <v>5595.228981147549</v>
       </c>
       <c r="X34">
-        <v>0.00508514497408817</v>
+        <v>5085.14497408817</v>
       </c>
       <c r="Y34">
-        <v>0.005150053966766877</v>
+        <v>5150.053966766876</v>
       </c>
       <c r="Z34">
         <v>0.2941983552815177</v>
@@ -3309,16 +3309,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V35">
-        <v>0.00661200363139354</v>
+        <v>6612.00363139354</v>
       </c>
       <c r="W35">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X35">
-        <v>0.00611099971677342</v>
+        <v>6110.99971677342</v>
       </c>
       <c r="Y35">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z35">
         <v>0.1492398017836711</v>
@@ -3392,16 +3392,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V36">
-        <v>0.006284261713154321</v>
+        <v>6284.26171315432</v>
       </c>
       <c r="W36">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X36">
-        <v>0.00529500221024781</v>
+        <v>5295.00221024781</v>
       </c>
       <c r="Y36">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z36">
         <v>-0.04956771600715904</v>
@@ -3475,16 +3475,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V37">
-        <v>0.0067083473270421</v>
+        <v>6708.3473270421</v>
       </c>
       <c r="W37">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X37">
-        <v>0.00643089618773373</v>
+        <v>6430.89618773373</v>
       </c>
       <c r="Y37">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z37">
         <v>0.0674837607415486</v>
@@ -3558,16 +3558,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V38">
-        <v>0.00610506181475701</v>
+        <v>6105.06181475701</v>
       </c>
       <c r="W38">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X38">
-        <v>0.00575840057666136</v>
+        <v>5758.40057666136</v>
       </c>
       <c r="Y38">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z38">
         <v>-0.08993057199843812</v>
@@ -3641,16 +3641,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V39">
-        <v>0.00487437595793455</v>
+        <v>4874.37595793455</v>
       </c>
       <c r="W39">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X39">
-        <v>0.00505320555537643</v>
+        <v>5053.20555537643</v>
       </c>
       <c r="Y39">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z39">
         <v>-0.2015845038370744</v>
@@ -3724,16 +3724,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V40">
-        <v>0.00474385058581087</v>
+        <v>4743.85058581087</v>
       </c>
       <c r="W40">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X40">
-        <v>0.00436930508934216</v>
+        <v>4369.30508934216</v>
       </c>
       <c r="Y40">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z40">
         <v>-0.02677786310496</v>
@@ -3807,16 +3807,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V41">
-        <v>0.00472837840069667</v>
+        <v>4728.37840069667</v>
       </c>
       <c r="W41">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X41">
-        <v>0.00530651142341538</v>
+        <v>5306.51142341538</v>
       </c>
       <c r="Y41">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z41">
         <v>-0.003261524543053396</v>
@@ -3890,16 +3890,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V42">
-        <v>0.00522263795498985</v>
+        <v>5222.63795498985</v>
       </c>
       <c r="W42">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X42">
-        <v>0.00614020989661176</v>
+        <v>6140.20989661176</v>
       </c>
       <c r="Y42">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z42">
         <v>0.104530456830688</v>
@@ -3973,16 +3973,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V43">
-        <v>0.00511500769629616</v>
+        <v>5115.00769629616</v>
       </c>
       <c r="W43">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X43">
-        <v>0.00420925829321361</v>
+        <v>4209.25829321361</v>
       </c>
       <c r="Y43">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z43">
         <v>-0.02060840893458005</v>
@@ -4056,16 +4056,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V44">
-        <v>0.00418378869342489</v>
+        <v>4183.78869342489</v>
       </c>
       <c r="W44">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X44">
-        <v>0.00287068276205765</v>
+        <v>2870.68276205765</v>
       </c>
       <c r="Y44">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z44">
         <v>-0.1820562271187934</v>
@@ -4139,16 +4139,16 @@
         <v>206.9287456798658</v>
       </c>
       <c r="V45">
-        <v>0.00598062621561352</v>
+        <v>5980.62621561352</v>
       </c>
       <c r="W45">
-        <v>0.005505303635555771</v>
+        <v>5505.303635555771</v>
       </c>
       <c r="X45">
-        <v>0.004621989505397011</v>
+        <v>4621.98950539701</v>
       </c>
       <c r="Y45">
-        <v>0.005106041928802756</v>
+        <v>5106.041928802756</v>
       </c>
       <c r="Z45">
         <v>0.4294761647528909</v>
@@ -4204,16 +4204,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V46">
-        <v>0.00693119550018943</v>
+        <v>6931.19550018943</v>
       </c>
       <c r="W46">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X46">
-        <v>0.006190889309492209</v>
+        <v>6190.88930949221</v>
       </c>
       <c r="Y46">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z46">
         <v>0.2084357881009724</v>
@@ -4287,16 +4287,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V47">
-        <v>0.00609899065022259</v>
+        <v>6098.99065022259</v>
       </c>
       <c r="W47">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X47">
-        <v>0.00561356490469029</v>
+        <v>5613.56490469029</v>
       </c>
       <c r="Y47">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z47">
         <v>-0.1200665671519575</v>
@@ -4370,16 +4370,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V48">
-        <v>0.00728403247125146</v>
+        <v>7284.03247125146</v>
       </c>
       <c r="W48">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X48">
-        <v>0.00647208368198496</v>
+        <v>6472.08368198496</v>
       </c>
       <c r="Y48">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z48">
         <v>0.194301301476109</v>
@@ -4453,16 +4453,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V49">
-        <v>0.00633455970651588</v>
+        <v>6334.55970651588</v>
       </c>
       <c r="W49">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X49">
-        <v>0.00542940700205123</v>
+        <v>5429.40700205123</v>
       </c>
       <c r="Y49">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z49">
         <v>-0.1303498808500578</v>
@@ -4536,16 +4536,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V50">
-        <v>0.00465510712341418</v>
+        <v>4655.10712341418</v>
       </c>
       <c r="W50">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X50">
-        <v>0.00495958004793761</v>
+        <v>4959.58004793761</v>
       </c>
       <c r="Y50">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z50">
         <v>-0.265125385332492</v>
@@ -4619,16 +4619,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V51">
-        <v>0.004762100663508261</v>
+        <v>4762.10066350826</v>
       </c>
       <c r="W51">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X51">
-        <v>0.00452877828719588</v>
+        <v>4528.77828719588</v>
       </c>
       <c r="Y51">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z51">
         <v>0.02298411986180215</v>
@@ -4702,16 +4702,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V52">
-        <v>0.00480694064605486</v>
+        <v>4806.94064605486</v>
       </c>
       <c r="W52">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X52">
-        <v>0.00546471660634492</v>
+        <v>5464.71660634492</v>
       </c>
       <c r="Y52">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z52">
         <v>0.009416008966422362</v>
@@ -4785,16 +4785,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V53">
-        <v>0.00451061425195751</v>
+        <v>4510.61425195751</v>
       </c>
       <c r="W53">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X53">
-        <v>0.00590253633411875</v>
+        <v>5902.53633411875</v>
       </c>
       <c r="Y53">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z53">
         <v>-0.06164552798057754</v>
@@ -4868,16 +4868,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V54">
-        <v>0.00532895664831211</v>
+        <v>5328.95664831211</v>
       </c>
       <c r="W54">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X54">
-        <v>0.00415639371543155</v>
+        <v>4156.39371543155</v>
       </c>
       <c r="Y54">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z54">
         <v>0.1814259323992198</v>
@@ -4951,16 +4951,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V55">
-        <v>0.00458565418896599</v>
+        <v>4585.65418896599</v>
       </c>
       <c r="W55">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X55">
-        <v>0.00304330991416957</v>
+        <v>3043.30991416957</v>
       </c>
       <c r="Y55">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z55">
         <v>-0.1394836753985516</v>
@@ -5034,16 +5034,16 @@
         <v>227.8606912079541</v>
       </c>
       <c r="V56">
-        <v>0.00621358367119202</v>
+        <v>6213.58367119202</v>
       </c>
       <c r="W56">
-        <v>0.005591975956507663</v>
+        <v>5591.975956507663</v>
       </c>
       <c r="X56">
-        <v>0.0048046688469924</v>
+        <v>4804.6688469924</v>
       </c>
       <c r="Y56">
-        <v>0.005142357150037215</v>
+        <v>5142.357150037215</v>
       </c>
       <c r="Z56">
         <v>0.3550048510293595</v>
@@ -5099,16 +5099,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V57">
-        <v>0.00688783378173856</v>
+        <v>6887.83378173856</v>
       </c>
       <c r="W57">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X57">
-        <v>0.00614772268515052</v>
+        <v>6147.72268515052</v>
       </c>
       <c r="Y57">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z57">
         <v>0.2253658613365876</v>
@@ -5182,16 +5182,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V58">
-        <v>0.00606508623481305</v>
+        <v>6065.08623481305</v>
       </c>
       <c r="W58">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X58">
-        <v>0.00557456870850665</v>
+        <v>5574.56870850665</v>
       </c>
       <c r="Y58">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z58">
         <v>-0.1194493904755407</v>
@@ -5265,16 +5265,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V59">
-        <v>0.00681259172620597</v>
+        <v>6812.59172620597</v>
       </c>
       <c r="W59">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X59">
-        <v>0.00638475874541589</v>
+        <v>6384.75874541589</v>
       </c>
       <c r="Y59">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z59">
         <v>0.1232472981344115</v>
@@ -5348,16 +5348,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V60">
-        <v>0.00654953658150255</v>
+        <v>6549.53658150255</v>
       </c>
       <c r="W60">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X60">
-        <v>0.00541265047575794</v>
+        <v>5412.65047575794</v>
       </c>
       <c r="Y60">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z60">
         <v>-0.03861307932068303</v>
@@ -5431,16 +5431,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V61">
-        <v>0.00547167724864759</v>
+        <v>5471.67724864759</v>
       </c>
       <c r="W61">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X61">
-        <v>0.00521405469060508</v>
+        <v>5214.05469060508</v>
       </c>
       <c r="Y61">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z61">
         <v>-0.1645703202725962</v>
@@ -5514,16 +5514,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V62">
-        <v>0.00482673837918025</v>
+        <v>4826.73837918025</v>
       </c>
       <c r="W62">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X62">
-        <v>0.00453770713776242</v>
+        <v>4537.70713776242</v>
       </c>
       <c r="Y62">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z62">
         <v>-0.1178685876669254</v>
@@ -5597,16 +5597,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V63">
-        <v>0.00470999104809569</v>
+        <v>4709.99104809569</v>
       </c>
       <c r="W63">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X63">
-        <v>0.00531427678521455</v>
+        <v>5314.27678521455</v>
       </c>
       <c r="Y63">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z63">
         <v>-0.02418762359031945</v>
@@ -5680,16 +5680,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V64">
-        <v>0.004756549665022559</v>
+        <v>4756.54966502256</v>
       </c>
       <c r="W64">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X64">
-        <v>0.00511799751444447</v>
+        <v>5117.99751444447</v>
       </c>
       <c r="Y64">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z64">
         <v>0.009885075460110304</v>
@@ -5763,16 +5763,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V65">
-        <v>0.00498809828535289</v>
+        <v>4988.09828535289</v>
       </c>
       <c r="W65">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X65">
-        <v>0.00408188861547836</v>
+        <v>4081.88861547836</v>
       </c>
       <c r="Y65">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z65">
         <v>0.04867995430238659</v>
@@ -5846,16 +5846,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V66">
-        <v>0.00448387983508466</v>
+        <v>4483.87983508466</v>
       </c>
       <c r="W66">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X66">
-        <v>0.00304800896937878</v>
+        <v>3048.00896937878</v>
       </c>
       <c r="Y66">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z66">
         <v>-0.1010843053651976</v>
@@ -5929,16 +5929,16 @@
         <v>225.8105631121805</v>
       </c>
       <c r="V67">
-        <v>0.00665689925692856</v>
+        <v>6656.89925692856</v>
       </c>
       <c r="W67">
-        <v>0.005655352912961121</v>
+        <v>5655.352912961121</v>
       </c>
       <c r="X67">
-        <v>0.005305534194369761</v>
+        <v>5305.53419436976</v>
       </c>
       <c r="Y67">
-        <v>0.005103560774734947</v>
+        <v>5103.560774734948</v>
       </c>
       <c r="Z67">
         <v>0.4846292723638237</v>
@@ -5994,16 +5994,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V68">
-        <v>0.006903182426899759</v>
+        <v>6903.18242689976</v>
       </c>
       <c r="W68">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X68">
-        <v>0.00646904673899306</v>
+        <v>6469.04673899306</v>
       </c>
       <c r="Y68">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z68">
         <v>0.2162164594338003</v>
@@ -6077,16 +6077,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V69">
-        <v>0.00716783943416908</v>
+        <v>7167.83943416908</v>
       </c>
       <c r="W69">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X69">
-        <v>0.00567944981900252</v>
+        <v>5679.44981900252</v>
       </c>
       <c r="Y69">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z69">
         <v>0.03833840552120238</v>
@@ -6160,16 +6160,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V70">
-        <v>0.00643848058298151</v>
+        <v>6438.48058298151</v>
       </c>
       <c r="W70">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X70">
-        <v>0.006051149649082791</v>
+        <v>6051.14964908279</v>
       </c>
       <c r="Y70">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z70">
         <v>-0.1017543512080805</v>
@@ -6243,16 +6243,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V71">
-        <v>0.00594018774266843</v>
+        <v>5940.18774266843</v>
       </c>
       <c r="W71">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X71">
-        <v>0.00542812793909097</v>
+        <v>5428.12793909097</v>
       </c>
       <c r="Y71">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z71">
         <v>-0.0773929242918262</v>
@@ -6326,16 +6326,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V72">
-        <v>0.00512097062967428</v>
+        <v>5120.97062967428</v>
       </c>
       <c r="W72">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X72">
-        <v>0.00511222267671636</v>
+        <v>5112.22267671636</v>
       </c>
       <c r="Y72">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z72">
         <v>-0.1379109800031579</v>
@@ -6409,16 +6409,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V73">
-        <v>0.00468332384647809</v>
+        <v>4683.32384647809</v>
       </c>
       <c r="W73">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X73">
-        <v>0.00447552632780996</v>
+        <v>4475.52632780996</v>
       </c>
       <c r="Y73">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z73">
         <v>-0.08546168584919744</v>
@@ -6492,16 +6492,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V74">
-        <v>0.00493849566492243</v>
+        <v>4938.49566492243</v>
       </c>
       <c r="W74">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X74">
-        <v>0.00561582177633401</v>
+        <v>5615.82177633401</v>
       </c>
       <c r="Y74">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z74">
         <v>0.05448519615747527</v>
@@ -6575,16 +6575,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V75">
-        <v>0.00494738371992442</v>
+        <v>4947.38371992442</v>
       </c>
       <c r="W75">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X75">
-        <v>0.00569671311157014</v>
+        <v>5696.71311157014</v>
       </c>
       <c r="Y75">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z75">
         <v>0.001799749479405532</v>
@@ -6658,16 +6658,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V76">
-        <v>0.00531689697912949</v>
+        <v>5316.89697912949</v>
       </c>
       <c r="W76">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X76">
-        <v>0.00436220314512317</v>
+        <v>4362.20314512317</v>
       </c>
       <c r="Y76">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z76">
         <v>0.07468861930335891</v>
@@ -6741,16 +6741,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V77">
-        <v>0.00447062595853963</v>
+        <v>4470.62595853963</v>
       </c>
       <c r="W77">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X77">
-        <v>0.00307948624555134</v>
+        <v>3079.48624555134</v>
       </c>
       <c r="Y77">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z77">
         <v>-0.159166337792841</v>
@@ -6824,16 +6824,16 @@
         <v>238.9676028030524</v>
       </c>
       <c r="V78">
-        <v>0.00671050330465365</v>
+        <v>6710.50330465365</v>
       </c>
       <c r="W78">
-        <v>0.00569435366273098</v>
+        <v>5694.35366273098</v>
       </c>
       <c r="X78">
-        <v>0.005264264885443941</v>
+        <v>5264.26488544394</v>
       </c>
       <c r="Y78">
-        <v>0.005203092028610751</v>
+        <v>5203.092028610751</v>
       </c>
       <c r="Z78">
         <v>0.5010209681790725</v>
@@ -6889,16 +6889,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V79">
-        <v>0.00736022415345869</v>
+        <v>7360.22415345869</v>
       </c>
       <c r="W79">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X79">
-        <v>0.00666821845106979</v>
+        <v>6668.21845106979</v>
       </c>
       <c r="Y79">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z79">
         <v>0.2907784327640566</v>
@@ -6972,16 +6972,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V80">
-        <v>0.00658204246396268</v>
+        <v>6582.04246396268</v>
       </c>
       <c r="W80">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X80">
-        <v>0.00545562985136555</v>
+        <v>5455.62985136555</v>
       </c>
       <c r="Y80">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z80">
         <v>-0.1057279877991664</v>
@@ -7055,16 +7055,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V81">
-        <v>0.00650479719949826</v>
+        <v>6504.79719949826</v>
       </c>
       <c r="W81">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X81">
-        <v>0.00630009775346396</v>
+        <v>6300.09775346396</v>
       </c>
       <c r="Y81">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z81">
         <v>-0.01173575905767021</v>
@@ -7138,16 +7138,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V82">
-        <v>0.00590922652529284</v>
+        <v>5909.22652529284</v>
       </c>
       <c r="W82">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X82">
-        <v>0.005291574925704029</v>
+        <v>5291.57492570403</v>
       </c>
       <c r="Y82">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z82">
         <v>-0.09155868445081705</v>
@@ -7221,16 +7221,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V83">
-        <v>0.00474269435903571</v>
+        <v>4742.69435903571</v>
       </c>
       <c r="W83">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X83">
-        <v>0.00513859291437999</v>
+        <v>5138.59291437999</v>
       </c>
       <c r="Y83">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z83">
         <v>-0.1974086052149306</v>
@@ -7304,16 +7304,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V84">
-        <v>0.00521670570615667</v>
+        <v>5216.70570615667</v>
       </c>
       <c r="W84">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X84">
-        <v>0.00449433909402706</v>
+        <v>4494.33909402706</v>
       </c>
       <c r="Y84">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z84">
         <v>0.09994558182267888</v>
@@ -7387,16 +7387,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V85">
-        <v>0.00477941860953737</v>
+        <v>4779.41860953737</v>
       </c>
       <c r="W85">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X85">
-        <v>0.005648669726035669</v>
+        <v>5648.66972603567</v>
       </c>
       <c r="Y85">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z85">
         <v>-0.08382437523803987</v>
@@ -7470,16 +7470,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V86">
-        <v>0.0047169743746086</v>
+        <v>4716.9743746086</v>
       </c>
       <c r="W86">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X86">
-        <v>0.00563355557580762</v>
+        <v>5633.55557580762</v>
       </c>
       <c r="Y86">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z86">
         <v>-0.01306523659680325</v>
@@ -7553,16 +7553,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V87">
-        <v>0.00515059292141893</v>
+        <v>5150.59292141893</v>
       </c>
       <c r="W87">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X87">
-        <v>0.00400297349660014</v>
+        <v>4002.97349660014</v>
       </c>
       <c r="Y87">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z87">
         <v>0.09192726361722303</v>
@@ -7636,16 +7636,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V88">
-        <v>0.00464140861785152</v>
+        <v>4641.40861785152</v>
       </c>
       <c r="W88">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X88">
-        <v>0.00325225543423215</v>
+        <v>3252.25543423215</v>
       </c>
       <c r="Y88">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z88">
         <v>-0.09885935684218961</v>
@@ -7719,16 +7719,16 @@
         <v>244.1932305913233</v>
       </c>
       <c r="V89">
-        <v>0.00755591888440658</v>
+        <v>7555.91888440658</v>
       </c>
       <c r="W89">
-        <v>0.005741818528657077</v>
+        <v>5741.818528657077</v>
       </c>
       <c r="X89">
-        <v>0.005248732774660939</v>
+        <v>5248.73277466094</v>
       </c>
       <c r="Y89">
-        <v>0.005194058181576991</v>
+        <v>5194.058181576991</v>
       </c>
       <c r="Z89">
         <v>0.6279365827316814</v>
@@ -7784,16 +7784,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V90">
-        <v>0.00731830102529294</v>
+        <v>7318.30102529294</v>
       </c>
       <c r="W90">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X90">
-        <v>0.00632311107972037</v>
+        <v>6323.11107972037</v>
       </c>
       <c r="Y90">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z90">
         <v>0.2086554152752245</v>
@@ -7867,16 +7867,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V91">
-        <v>0.00657433052894782</v>
+        <v>6574.33052894782</v>
       </c>
       <c r="W91">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X91">
-        <v>0.00578406994730814</v>
+        <v>5784.06994730814</v>
       </c>
       <c r="Y91">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z91">
         <v>-0.1016589087786723</v>
@@ -7950,16 +7950,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V92">
-        <v>0.00629134538835408</v>
+        <v>6291.34538835408</v>
       </c>
       <c r="W92">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X92">
-        <v>0.00575282076073566</v>
+        <v>5752.82076073566</v>
       </c>
       <c r="Y92">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z92">
         <v>-0.04304394787388799</v>
@@ -8033,16 +8033,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V93">
-        <v>0.005402905004518551</v>
+        <v>5402.90500451855</v>
       </c>
       <c r="W93">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X93">
-        <v>0.00531871417597703</v>
+        <v>5318.71417597703</v>
       </c>
       <c r="Y93">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z93">
         <v>-0.1412162787120419</v>
@@ -8116,16 +8116,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V94">
-        <v>0.004896373548877991</v>
+        <v>4896.37354887799</v>
       </c>
       <c r="W94">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X94">
-        <v>0.00507884348935178</v>
+        <v>5078.84348935178</v>
       </c>
       <c r="Y94">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z94">
         <v>-0.0937516864014708</v>
@@ -8199,16 +8199,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V95">
-        <v>0.00478078168676988</v>
+        <v>4780.78168676988</v>
       </c>
       <c r="W95">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X95">
-        <v>0.00441603620818464</v>
+        <v>4416.03620818464</v>
       </c>
       <c r="Y95">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z95">
         <v>-0.02360764777323787</v>
@@ -8282,16 +8282,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V96">
-        <v>0.0050281607822665</v>
+        <v>5028.1607822665</v>
       </c>
       <c r="W96">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X96">
-        <v>0.00579301045127984</v>
+        <v>5793.01045127984</v>
       </c>
       <c r="Y96">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z96">
         <v>0.05174448692798617</v>
@@ -8365,16 +8365,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V97">
-        <v>0.004833414375727379</v>
+        <v>4833.41437572738</v>
       </c>
       <c r="W97">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X97">
-        <v>0.00484834619922436</v>
+        <v>4848.34619922436</v>
       </c>
       <c r="Y97">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z97">
         <v>-0.03873114145950929</v>
@@ -8448,16 +8448,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V98">
-        <v>0.00547466307489423</v>
+        <v>5474.66307489423</v>
       </c>
       <c r="W98">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X98">
-        <v>0.00396169124576404</v>
+        <v>3961.69124576404</v>
       </c>
       <c r="Y98">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z98">
         <v>0.1326699201266701</v>
@@ -8531,16 +8531,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V99">
-        <v>0.00444210507813407</v>
+        <v>4442.10507813407</v>
       </c>
       <c r="W99">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X99">
-        <v>0.00389528479862121</v>
+        <v>3895.28479862121</v>
       </c>
       <c r="Y99">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z99">
         <v>-0.188606674535877</v>
@@ -8614,16 +8614,16 @@
         <v>233.2044337283513</v>
       </c>
       <c r="V100">
-        <v>0.00715274614168193</v>
+        <v>7152.74614168193</v>
       </c>
       <c r="W100">
-        <v>0.005654102421405943</v>
+        <v>5654.102421405943</v>
       </c>
       <c r="X100">
-        <v>0.00567516181397285</v>
+        <v>5675.16181397285</v>
       </c>
       <c r="Y100">
-        <v>0.005167917288194538</v>
+        <v>5167.917288194538</v>
       </c>
       <c r="Z100">
         <v>0.6102154307179242</v>
@@ -8679,16 +8679,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V101">
-        <v>0.007353357895771229</v>
+        <v>7353.35789577123</v>
       </c>
       <c r="W101">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X101">
-        <v>0.006199954565752779</v>
+        <v>6199.95456575278</v>
       </c>
       <c r="Y101">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z101">
         <v>0.2521179904724522</v>
@@ -8762,16 +8762,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V102">
-        <v>0.00663102567268779</v>
+        <v>6631.02567268779</v>
       </c>
       <c r="W102">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X102">
-        <v>0.00582442620282346</v>
+        <v>5824.42620282346</v>
       </c>
       <c r="Y102">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z102">
         <v>-0.09823161517799084</v>
@@ -8845,16 +8845,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V103">
-        <v>0.005837006398395499</v>
+        <v>5837.0063983955</v>
       </c>
       <c r="W103">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X103">
-        <v>0.006438106442165891</v>
+        <v>6438.10644216589</v>
       </c>
       <c r="Y103">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z103">
         <v>-0.1197430553711679</v>
@@ -8928,16 +8928,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V104">
-        <v>0.00558393037814565</v>
+        <v>5583.93037814565</v>
       </c>
       <c r="W104">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X104">
-        <v>0.00511887497675149</v>
+        <v>5118.87497675149</v>
       </c>
       <c r="Y104">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z104">
         <v>-0.04335715998519651</v>
@@ -9011,16 +9011,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V105">
-        <v>0.00487995165320697</v>
+        <v>4879.95165320697</v>
       </c>
       <c r="W105">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X105">
-        <v>0.00486016673696453</v>
+        <v>4860.16673696453</v>
       </c>
       <c r="Y105">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z105">
         <v>-0.1260722604447053</v>
@@ -9094,16 +9094,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V106">
-        <v>0.00462677469127344</v>
+        <v>4626.77469127344</v>
       </c>
       <c r="W106">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X106">
-        <v>0.00466368748125391</v>
+        <v>4663.68748125391</v>
       </c>
       <c r="Y106">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z106">
         <v>-0.05188103897856222</v>
@@ -9177,16 +9177,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V107">
-        <v>0.0050738111398448</v>
+        <v>5073.8111398448</v>
       </c>
       <c r="W107">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X107">
-        <v>0.00598506379845051</v>
+        <v>5985.06379845051</v>
       </c>
       <c r="Y107">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z107">
         <v>0.09661945489036139</v>
@@ -9260,16 +9260,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V108">
-        <v>0.00511253605996848</v>
+        <v>5112.53605996848</v>
       </c>
       <c r="W108">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X108">
-        <v>0.00475897035569549</v>
+        <v>4758.97035569549</v>
       </c>
       <c r="Y108">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z108">
         <v>0.007632314064583978</v>
@@ -9343,16 +9343,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V109">
-        <v>0.00561089126928224</v>
+        <v>5610.89126928224</v>
       </c>
       <c r="W109">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X109">
-        <v>0.00389146345291231</v>
+        <v>3891.46345291231</v>
       </c>
       <c r="Y109">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z109">
         <v>0.09747710401808529</v>
@@ -9426,16 +9426,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V110">
-        <v>0.00451042707247351</v>
+        <v>4510.42707247351</v>
       </c>
       <c r="W110">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X110">
-        <v>0.00385219196798159</v>
+        <v>3852.19196798159</v>
       </c>
       <c r="Y110">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z110">
         <v>-0.1961300164259829</v>
@@ -9509,16 +9509,16 @@
         <v>237.0739683137839</v>
       </c>
       <c r="V111">
-        <v>0.006723780112371389</v>
+        <v>6723.78011237139</v>
       </c>
       <c r="W111">
-        <v>0.005631226576674636</v>
+        <v>5631.226576674636</v>
       </c>
       <c r="X111">
-        <v>0.00534496652081321</v>
+        <v>5344.96652081321</v>
       </c>
       <c r="Y111">
-        <v>0.005176170227415016</v>
+        <v>5176.170227415016</v>
       </c>
       <c r="Z111">
         <v>0.4907191723386144</v>
@@ -9574,16 +9574,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V112">
-        <v>0.00681841212183733</v>
+        <v>6818.41212183733</v>
       </c>
       <c r="W112">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X112">
-        <v>0.00609067707517758</v>
+        <v>6090.67707517758</v>
       </c>
       <c r="Y112">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z112">
         <v>0.09640695291628454</v>
@@ -9657,16 +9657,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V113">
-        <v>0.00699470706375033</v>
+        <v>6994.70706375033</v>
       </c>
       <c r="W113">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X113">
-        <v>0.00571158641456206</v>
+        <v>5711.58641456206</v>
       </c>
       <c r="Y113">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z113">
         <v>0.02585571812950116</v>
@@ -9740,16 +9740,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V114">
-        <v>0.00546069812802098</v>
+        <v>5460.69812802098</v>
       </c>
       <c r="W114">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X114">
-        <v>0.00622491355290388</v>
+        <v>6224.91355290388</v>
       </c>
       <c r="Y114">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z114">
         <v>-0.2193099613390908</v>
@@ -9823,16 +9823,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V115">
-        <v>0.0053047203887012</v>
+        <v>5304.7203887012</v>
       </c>
       <c r="W115">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X115">
-        <v>0.00502754093715553</v>
+        <v>5027.54093715553</v>
       </c>
       <c r="Y115">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z115">
         <v>-0.02856369930419655</v>
@@ -9906,16 +9906,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V116">
-        <v>0.00425891729289603</v>
+        <v>4258.91729289603</v>
       </c>
       <c r="W116">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X116">
-        <v>0.00494737380775459</v>
+        <v>4947.37380775459</v>
       </c>
       <c r="Y116">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z116">
         <v>-0.1971457530603651</v>
@@ -9989,16 +9989,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V117">
-        <v>0.00505643183049269</v>
+        <v>5056.43183049269</v>
       </c>
       <c r="W117">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X117">
-        <v>0.00473155853084878</v>
+        <v>4731.55853084878</v>
       </c>
       <c r="Y117">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z117">
         <v>0.1872575781001742</v>
@@ -10072,16 +10072,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V118">
-        <v>0.00482566488741333</v>
+        <v>4825.66488741333</v>
       </c>
       <c r="W118">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X118">
-        <v>0.00637826649800118</v>
+        <v>6378.26649800118</v>
       </c>
       <c r="Y118">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z118">
         <v>-0.04563829807567577</v>
@@ -10155,16 +10155,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V119">
-        <v>0.005506867914858111</v>
+        <v>5506.86791485811</v>
       </c>
       <c r="W119">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X119">
-        <v>0.00448746001978346</v>
+        <v>4487.46001978346</v>
       </c>
       <c r="Y119">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z119">
         <v>0.1411625223337714</v>
@@ -10238,16 +10238,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V120">
-        <v>0.0061211746396576</v>
+        <v>6121.1746396576</v>
       </c>
       <c r="W120">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X120">
-        <v>0.00357486898630027</v>
+        <v>3574.86898630027</v>
       </c>
       <c r="Y120">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z120">
         <v>0.1115528344418839</v>
@@ -10321,16 +10321,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V121">
-        <v>0.004662040879050399</v>
+        <v>4662.0408790504</v>
       </c>
       <c r="W121">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X121">
-        <v>0.0044033408969418</v>
+        <v>4403.3408969418</v>
       </c>
       <c r="Y121">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z121">
         <v>-0.238374796751236</v>
@@ -10404,16 +10404,16 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V122">
-        <v>0.00632523575329086</v>
+        <v>6325.23575329086</v>
       </c>
       <c r="W122">
-        <v>0.005575897354542624</v>
+        <v>5575.897354542623</v>
       </c>
       <c r="X122">
-        <v>0.00606452741786691</v>
+        <v>6064.52741786691</v>
       </c>
       <c r="Y122">
-        <v>0.00524019219429964</v>
+        <v>5240.192194299641</v>
       </c>
       <c r="Z122">
         <v>0.3567525290724676</v>
@@ -10469,16 +10469,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V123">
-        <v>0.00697339740655999</v>
+        <v>6973.39740655999</v>
       </c>
       <c r="W123">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X123">
-        <v>0.00649255120756501</v>
+        <v>6492.55120756501</v>
       </c>
       <c r="Y123">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z123">
         <v>0.157153587321696</v>
@@ -10552,16 +10552,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V124">
-        <v>0.00705495862848423</v>
+        <v>7054.95862848423</v>
       </c>
       <c r="W124">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X124">
-        <v>0.00605742777885964</v>
+        <v>6057.42777885964</v>
       </c>
       <c r="Y124">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z124">
         <v>0.01169605246468741</v>
@@ -10635,16 +10635,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V125">
-        <v>0.00548631712769005</v>
+        <v>5486.31712769005</v>
       </c>
       <c r="W125">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X125">
-        <v>0.00595737805653081</v>
+        <v>5957.37805653081</v>
       </c>
       <c r="Y125">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z125">
         <v>-0.2223459531655971</v>
@@ -10718,16 +10718,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V126">
-        <v>0.00489066126128942</v>
+        <v>4890.66126128942</v>
       </c>
       <c r="W126">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X126">
-        <v>0.004641744545881931</v>
+        <v>4641.74454588193</v>
       </c>
       <c r="Y126">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z126">
         <v>-0.1085711694269895</v>
@@ -10801,16 +10801,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V127">
-        <v>0.00368045650967716</v>
+        <v>3680.45650967716</v>
       </c>
       <c r="W127">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X127">
-        <v>0.0048554435403952</v>
+        <v>4855.4435403952</v>
       </c>
       <c r="Y127">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z127">
         <v>-0.2474521719979417</v>
@@ -10884,16 +10884,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V128">
-        <v>0.0049895028814981</v>
+        <v>4989.5028814981</v>
       </c>
       <c r="W128">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X128">
-        <v>0.00514851371860231</v>
+        <v>5148.51371860231</v>
       </c>
       <c r="Y128">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z128">
         <v>0.3556750007448848</v>
@@ -10967,16 +10967,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V129">
-        <v>0.00491787707307164</v>
+        <v>4917.87707307164</v>
       </c>
       <c r="W129">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X129">
-        <v>0.00639783985189199</v>
+        <v>6397.83985189199</v>
       </c>
       <c r="Y129">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z129">
         <v>-0.01435529954137527</v>
@@ -11050,16 +11050,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V130">
-        <v>0.00570092418809841</v>
+        <v>5700.92418809841</v>
       </c>
       <c r="W130">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X130">
-        <v>0.004535344579386751</v>
+        <v>4535.34457938675</v>
       </c>
       <c r="Y130">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z130">
         <v>0.1592246213949569</v>
@@ -11133,16 +11133,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V131">
-        <v>0.00565254682956926</v>
+        <v>5652.54682956926</v>
       </c>
       <c r="W131">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X131">
-        <v>0.0035317381716411</v>
+        <v>3531.7381716411</v>
       </c>
       <c r="Y131">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z131">
         <v>-0.00848587999646544</v>
@@ -11216,16 +11216,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V132">
-        <v>0.00367835313522258</v>
+        <v>3678.35313522258</v>
       </c>
       <c r="W132">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X132">
-        <v>0.00435755412502467</v>
+        <v>4357.55412502467</v>
       </c>
       <c r="Y132">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z132">
         <v>-0.3492573797034989</v>
@@ -11263,16 +11263,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V133">
-        <v>0.00680048397084986</v>
+        <v>6800.48397084986</v>
       </c>
       <c r="W133">
-        <v>0.005438679910182791</v>
+        <v>5438.679910182791</v>
       </c>
       <c r="X133">
-        <v>0.00688002173009005</v>
+        <v>6880.02173009005</v>
       </c>
       <c r="Y133">
-        <v>0.005350505209624496</v>
+        <v>5350.505209624497</v>
       </c>
       <c r="Z133">
         <v>0.8487849645894201</v>

</xml_diff>